<commit_message>
Updated Schedule for revised CSC's
</commit_message>
<xml_diff>
--- a/Docs/FSAE Software Initial Development Schedule.xlsx
+++ b/Docs/FSAE Software Initial Development Schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>FSAE SOFTWARE TIMELINE</t>
   </si>
@@ -154,28 +154,34 @@
     <t>Input Observer CSC</t>
   </si>
   <si>
+    <t>- Data Management CSC</t>
+  </si>
+  <si>
+    <t>Data Management CSC</t>
+  </si>
+  <si>
     <t>- Telemetry GUI CSC</t>
   </si>
   <si>
     <t>Telemetry GUI CSC</t>
   </si>
   <si>
-    <t>- Traction Control CSC</t>
-  </si>
-  <si>
-    <t>Traction Control CSC</t>
-  </si>
-  <si>
-    <t>- Virtual Differential CSC</t>
-  </si>
-  <si>
-    <t>Virtual Differential CSC</t>
+    <t>- Traction Control CSU</t>
+  </si>
+  <si>
+    <t>Traction Control CSU</t>
+  </si>
+  <si>
+    <t>- Virtual Differential CSU</t>
+  </si>
+  <si>
+    <t>Virtual Differential CSU</t>
   </si>
   <si>
     <t>- Suspension Motor Controller CSC</t>
   </si>
   <si>
-    <t>Suspension Motor Controller CSC</t>
+    <t>Suspension Motor Controller CSU</t>
   </si>
   <si>
     <t>- Steering Wheel Unit Processor CSC</t>
@@ -202,22 +208,10 @@
     <t>Graphics Interface CSC</t>
   </si>
   <si>
-    <t>- Data Management CSC</t>
-  </si>
-  <si>
-    <t>Data Management CSC</t>
-  </si>
-  <si>
-    <t>- Suspension Kinematics CSC</t>
+    <t>- Suspension Kinematics CSU</t>
   </si>
   <si>
     <t>Suspension Kinematics CSC</t>
-  </si>
-  <si>
-    <t>- Cheating Mode CSC</t>
-  </si>
-  <si>
-    <t>Cheating Mode CSC</t>
   </si>
 </sst>
 </file>
@@ -228,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -449,6 +443,10 @@
       <sz val="9.0"/>
       <color rgb="FF38761D"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <name val="Corbel"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1027,7 +1025,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="184">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1479,6 +1477,17 @@
     <xf borderId="0" fillId="9" fontId="35" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="8" fontId="42" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="2" fontId="43" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="2" fontId="43" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="2" fontId="43" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="35" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="43" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="45" fillId="2" fontId="43" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="2" fontId="40" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1500,38 +1509,8 @@
     <xf borderId="45" fillId="2" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="28" fillId="2" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="21" fillId="2" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="25" fillId="2" fontId="40" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="40" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="45" fillId="2" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="29" fillId="2" fontId="41" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="41" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="41" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="24" fillId="2" fontId="41" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="26" fillId="2" fontId="41" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="46" fillId="8" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1584,6 +1563,7 @@
   <sheetPr>
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2862,25 +2842,25 @@
     <row r="23" ht="21.0" customHeight="1">
       <c r="A23" s="33"/>
       <c r="C23" s="64"/>
-      <c r="G23" s="139" t="s">
+      <c r="G23" s="157" t="s">
         <v>47</v>
       </c>
       <c r="H23" s="67"/>
-      <c r="I23" s="140"/>
-      <c r="J23" s="157"/>
-      <c r="K23" s="141"/>
-      <c r="L23" s="141"/>
-      <c r="M23" s="141"/>
-      <c r="N23" s="141"/>
-      <c r="O23" s="142"/>
-      <c r="P23" s="156" t="s">
+      <c r="I23" s="158"/>
+      <c r="J23" s="159"/>
+      <c r="K23" s="160"/>
+      <c r="L23" s="160"/>
+      <c r="M23" s="160"/>
+      <c r="N23" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="R23" s="158"/>
-      <c r="S23" s="141"/>
-      <c r="T23" s="141"/>
-      <c r="U23" s="141"/>
-      <c r="V23" s="142"/>
+      <c r="P23" s="159"/>
+      <c r="Q23" s="159"/>
+      <c r="R23" s="160"/>
+      <c r="S23" s="160"/>
+      <c r="T23" s="160"/>
+      <c r="U23" s="162"/>
+      <c r="V23" s="163"/>
       <c r="X23" s="145"/>
       <c r="Y23" s="146"/>
       <c r="Z23" s="146"/>
@@ -2915,7 +2895,7 @@
       </c>
       <c r="H24" s="67"/>
       <c r="I24" s="140"/>
-      <c r="J24" s="157"/>
+      <c r="J24" s="164"/>
       <c r="K24" s="141"/>
       <c r="L24" s="141"/>
       <c r="M24" s="141"/>
@@ -2924,7 +2904,8 @@
       <c r="P24" s="156" t="s">
         <v>50</v>
       </c>
-      <c r="S24" s="144"/>
+      <c r="R24" s="165"/>
+      <c r="S24" s="141"/>
       <c r="T24" s="141"/>
       <c r="U24" s="141"/>
       <c r="V24" s="142"/>
@@ -2962,7 +2943,7 @@
       </c>
       <c r="H25" s="67"/>
       <c r="I25" s="140"/>
-      <c r="J25" s="157"/>
+      <c r="J25" s="164"/>
       <c r="K25" s="141"/>
       <c r="L25" s="141"/>
       <c r="M25" s="141"/>
@@ -2971,7 +2952,7 @@
       <c r="P25" s="156" t="s">
         <v>52</v>
       </c>
-      <c r="S25" s="158"/>
+      <c r="S25" s="144"/>
       <c r="T25" s="141"/>
       <c r="U25" s="141"/>
       <c r="V25" s="142"/>
@@ -3009,18 +2990,17 @@
       </c>
       <c r="H26" s="67"/>
       <c r="I26" s="140"/>
-      <c r="J26" s="157"/>
+      <c r="J26" s="164"/>
       <c r="K26" s="141"/>
       <c r="L26" s="141"/>
       <c r="M26" s="141"/>
       <c r="N26" s="141"/>
-      <c r="O26" s="141"/>
-      <c r="P26" s="141"/>
-      <c r="Q26" s="142"/>
-      <c r="R26" s="156" t="s">
+      <c r="O26" s="142"/>
+      <c r="P26" s="156" t="s">
         <v>54</v>
       </c>
-      <c r="T26" s="144"/>
+      <c r="S26" s="165"/>
+      <c r="T26" s="141"/>
       <c r="U26" s="141"/>
       <c r="V26" s="142"/>
       <c r="X26" s="145"/>
@@ -3052,26 +3032,25 @@
     <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="33"/>
       <c r="C27" s="64"/>
-      <c r="G27" s="151" t="s">
+      <c r="G27" s="139" t="s">
         <v>55</v>
       </c>
       <c r="H27" s="67"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="153"/>
-      <c r="K27" s="154"/>
-      <c r="L27" s="154"/>
-      <c r="M27" s="154"/>
-      <c r="N27" s="153"/>
-      <c r="O27" s="153"/>
-      <c r="P27" s="154"/>
-      <c r="Q27" s="154"/>
-      <c r="R27" s="155"/>
-      <c r="S27" s="156" t="s">
+      <c r="I27" s="140"/>
+      <c r="J27" s="164"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="141"/>
+      <c r="N27" s="141"/>
+      <c r="O27" s="141"/>
+      <c r="P27" s="141"/>
+      <c r="Q27" s="142"/>
+      <c r="R27" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="T27" s="159"/>
-      <c r="U27" s="154"/>
-      <c r="V27" s="155"/>
+      <c r="T27" s="144"/>
+      <c r="U27" s="141"/>
+      <c r="V27" s="142"/>
       <c r="X27" s="145"/>
       <c r="Y27" s="146"/>
       <c r="Z27" s="146"/>
@@ -3110,15 +3089,15 @@
       <c r="K28" s="154"/>
       <c r="L28" s="154"/>
       <c r="M28" s="154"/>
-      <c r="N28" s="160"/>
-      <c r="O28" s="160"/>
-      <c r="P28" s="161"/>
+      <c r="N28" s="153"/>
+      <c r="O28" s="153"/>
+      <c r="P28" s="154"/>
       <c r="Q28" s="154"/>
       <c r="R28" s="155"/>
       <c r="S28" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="T28" s="98"/>
+      <c r="T28" s="166"/>
       <c r="U28" s="154"/>
       <c r="V28" s="155"/>
       <c r="X28" s="145"/>
@@ -3154,22 +3133,22 @@
         <v>59</v>
       </c>
       <c r="H29" s="67"/>
-      <c r="I29" s="162"/>
-      <c r="J29" s="160"/>
-      <c r="K29" s="161"/>
-      <c r="L29" s="161"/>
-      <c r="M29" s="161"/>
-      <c r="N29" s="160"/>
-      <c r="O29" s="160"/>
-      <c r="P29" s="161"/>
+      <c r="I29" s="152"/>
+      <c r="J29" s="153"/>
+      <c r="K29" s="154"/>
+      <c r="L29" s="154"/>
+      <c r="M29" s="154"/>
+      <c r="N29" s="167"/>
+      <c r="O29" s="167"/>
+      <c r="P29" s="168"/>
       <c r="Q29" s="154"/>
-      <c r="R29" s="154"/>
-      <c r="S29" s="155"/>
-      <c r="T29" s="156" t="s">
+      <c r="R29" s="155"/>
+      <c r="S29" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="U29" s="159"/>
-      <c r="V29" s="163"/>
+      <c r="T29" s="98"/>
+      <c r="U29" s="154"/>
+      <c r="V29" s="155"/>
       <c r="X29" s="145"/>
       <c r="Y29" s="146"/>
       <c r="Z29" s="146"/>
@@ -3203,22 +3182,22 @@
         <v>61</v>
       </c>
       <c r="H30" s="67"/>
-      <c r="I30" s="152"/>
-      <c r="J30" s="153"/>
-      <c r="K30" s="154"/>
-      <c r="L30" s="154"/>
-      <c r="M30" s="154"/>
-      <c r="N30" s="153"/>
-      <c r="O30" s="153"/>
-      <c r="P30" s="154"/>
+      <c r="I30" s="169"/>
+      <c r="J30" s="167"/>
+      <c r="K30" s="168"/>
+      <c r="L30" s="168"/>
+      <c r="M30" s="168"/>
+      <c r="N30" s="167"/>
+      <c r="O30" s="167"/>
+      <c r="P30" s="168"/>
       <c r="Q30" s="154"/>
       <c r="R30" s="154"/>
       <c r="S30" s="155"/>
       <c r="T30" s="156" t="s">
         <v>62</v>
       </c>
-      <c r="U30" s="164"/>
-      <c r="V30" s="165"/>
+      <c r="U30" s="166"/>
+      <c r="V30" s="170"/>
       <c r="X30" s="145"/>
       <c r="Y30" s="146"/>
       <c r="Z30" s="146"/>
@@ -3252,21 +3231,22 @@
         <v>63</v>
       </c>
       <c r="H31" s="67"/>
-      <c r="I31" s="140"/>
-      <c r="J31" s="157"/>
-      <c r="K31" s="141"/>
-      <c r="L31" s="141"/>
-      <c r="M31" s="141"/>
-      <c r="N31" s="141"/>
-      <c r="O31" s="141"/>
-      <c r="P31" s="141"/>
-      <c r="Q31" s="141"/>
-      <c r="R31" s="141"/>
-      <c r="S31" s="141"/>
-      <c r="T31" s="142"/>
-      <c r="U31" s="156" t="s">
+      <c r="I31" s="152"/>
+      <c r="J31" s="153"/>
+      <c r="K31" s="154"/>
+      <c r="L31" s="154"/>
+      <c r="M31" s="154"/>
+      <c r="N31" s="153"/>
+      <c r="O31" s="153"/>
+      <c r="P31" s="154"/>
+      <c r="Q31" s="154"/>
+      <c r="R31" s="154"/>
+      <c r="S31" s="155"/>
+      <c r="T31" s="156" t="s">
         <v>64</v>
       </c>
+      <c r="U31" s="166"/>
+      <c r="V31" s="171"/>
       <c r="X31" s="145"/>
       <c r="Y31" s="146"/>
       <c r="Z31" s="146"/>
@@ -3295,170 +3275,123 @@
     </row>
     <row r="32" ht="21.0" customHeight="1">
       <c r="A32" s="33"/>
-      <c r="C32" s="64"/>
-      <c r="G32" s="151" t="s">
+      <c r="C32" s="172"/>
+      <c r="D32" s="124"/>
+      <c r="E32" s="124"/>
+      <c r="F32" s="124"/>
+      <c r="G32" s="173" t="s">
         <v>65</v>
       </c>
-      <c r="H32" s="67"/>
-      <c r="I32" s="166"/>
-      <c r="J32" s="167"/>
-      <c r="K32" s="168"/>
-      <c r="L32" s="168"/>
-      <c r="M32" s="168"/>
-      <c r="N32" s="168"/>
-      <c r="O32" s="168"/>
-      <c r="P32" s="168"/>
-      <c r="Q32" s="168"/>
-      <c r="R32" s="168"/>
-      <c r="S32" s="168"/>
-      <c r="T32" s="169"/>
+      <c r="H32" s="174"/>
+      <c r="I32" s="175"/>
+      <c r="J32" s="176"/>
+      <c r="K32" s="177"/>
+      <c r="L32" s="177"/>
+      <c r="M32" s="177"/>
+      <c r="N32" s="177"/>
+      <c r="O32" s="177"/>
+      <c r="P32" s="177"/>
+      <c r="Q32" s="177"/>
+      <c r="R32" s="177"/>
+      <c r="S32" s="177"/>
+      <c r="T32" s="178"/>
       <c r="U32" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="X32" s="170"/>
-      <c r="Y32" s="171"/>
-      <c r="Z32" s="172"/>
-      <c r="AA32" s="172"/>
-      <c r="AB32" s="172"/>
-      <c r="AC32" s="172"/>
-      <c r="AD32" s="172"/>
-      <c r="AE32" s="172"/>
-      <c r="AF32" s="172"/>
-      <c r="AG32" s="172"/>
-      <c r="AH32" s="172"/>
-      <c r="AI32" s="172"/>
-      <c r="AJ32" s="172"/>
-      <c r="AK32" s="172"/>
-      <c r="AL32" s="173"/>
-      <c r="AM32" s="172"/>
-      <c r="AN32" s="172"/>
-      <c r="AO32" s="172"/>
-      <c r="AP32" s="172"/>
-      <c r="AQ32" s="172"/>
-      <c r="AR32" s="172"/>
-      <c r="AS32" s="174"/>
-      <c r="AT32" s="172"/>
-      <c r="AU32" s="174"/>
+      <c r="X32" s="179"/>
+      <c r="Y32" s="180"/>
+      <c r="Z32" s="180"/>
+      <c r="AA32" s="180"/>
+      <c r="AB32" s="180"/>
+      <c r="AC32" s="180"/>
+      <c r="AD32" s="180"/>
+      <c r="AE32" s="180"/>
+      <c r="AF32" s="180"/>
+      <c r="AG32" s="180"/>
+      <c r="AH32" s="180"/>
+      <c r="AI32" s="180"/>
+      <c r="AJ32" s="180"/>
+      <c r="AK32" s="180"/>
+      <c r="AL32" s="181"/>
+      <c r="AM32" s="182"/>
+      <c r="AN32" s="180"/>
+      <c r="AO32" s="180"/>
+      <c r="AP32" s="183"/>
+      <c r="AQ32" s="180"/>
+      <c r="AR32" s="180"/>
+      <c r="AS32" s="180"/>
+      <c r="AT32" s="180"/>
+      <c r="AU32" s="183"/>
       <c r="AV32" s="90"/>
     </row>
-    <row r="33" ht="21.0" customHeight="1">
-      <c r="A33" s="33"/>
-      <c r="C33" s="175"/>
-      <c r="D33" s="124"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="176" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" s="177"/>
-      <c r="I33" s="178"/>
-      <c r="J33" s="179"/>
-      <c r="K33" s="180"/>
-      <c r="L33" s="180"/>
-      <c r="M33" s="180"/>
-      <c r="N33" s="180"/>
-      <c r="O33" s="180"/>
-      <c r="P33" s="180"/>
-      <c r="Q33" s="180"/>
-      <c r="R33" s="180"/>
-      <c r="S33" s="180"/>
-      <c r="T33" s="181"/>
-      <c r="U33" s="156" t="s">
-        <v>68</v>
-      </c>
-      <c r="X33" s="182"/>
-      <c r="Y33" s="183"/>
-      <c r="Z33" s="183"/>
-      <c r="AA33" s="183"/>
-      <c r="AB33" s="183"/>
-      <c r="AC33" s="183"/>
-      <c r="AD33" s="183"/>
-      <c r="AE33" s="183"/>
-      <c r="AF33" s="183"/>
-      <c r="AG33" s="183"/>
-      <c r="AH33" s="183"/>
-      <c r="AI33" s="183"/>
-      <c r="AJ33" s="183"/>
-      <c r="AK33" s="183"/>
-      <c r="AL33" s="184"/>
-      <c r="AM33" s="185"/>
-      <c r="AN33" s="183"/>
-      <c r="AO33" s="183"/>
-      <c r="AP33" s="186"/>
-      <c r="AQ33" s="183"/>
-      <c r="AR33" s="183"/>
-      <c r="AS33" s="183"/>
-      <c r="AT33" s="183"/>
-      <c r="AU33" s="186"/>
-      <c r="AV33" s="90"/>
-    </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="62">
+    <mergeCell ref="D11:F20"/>
+    <mergeCell ref="U32:V32"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D21:F32"/>
+    <mergeCell ref="B21:B32"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="W11:W32"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="S18:V18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="U20:V20"/>
     <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="G24:H24"/>
+    <mergeCell ref="P24:Q24"/>
     <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="AE9:AH9"/>
-    <mergeCell ref="AI9:AM9"/>
-    <mergeCell ref="AN9:AQ9"/>
-    <mergeCell ref="AR9:AU9"/>
-    <mergeCell ref="V9:Z9"/>
-    <mergeCell ref="AA9:AD9"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D11:F20"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="D21:F33"/>
-    <mergeCell ref="B21:B33"/>
-    <mergeCell ref="W11:W33"/>
-    <mergeCell ref="AV11:AV33"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="B2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:AF2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:AB4"/>
     <mergeCell ref="I5:O5"/>
     <mergeCell ref="P5:AA5"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="U32:V32"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="S18:V18"/>
+    <mergeCell ref="AN9:AQ9"/>
+    <mergeCell ref="AR9:AU9"/>
+    <mergeCell ref="AV11:AV32"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="R16:S16"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="V9:Z9"/>
+    <mergeCell ref="AA9:AD9"/>
+    <mergeCell ref="AE9:AH9"/>
+    <mergeCell ref="AI9:AM9"/>
+    <mergeCell ref="L11:N11"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>